<commit_message>
agregada carpeta Chemistry para archivos orca, y datos de avances
</commit_message>
<xml_diff>
--- a/docs/textAvance.xlsx
+++ b/docs/textAvance.xlsx
@@ -1,43 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff2dc98e2a8f9132/University Proyect/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{B592493F-7676-4A14-9DC4-76C7A4973797}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{174778ED-BF3D-42A4-A245-062591C956B6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19545" windowHeight="8385" xr2:uid="{C6E18974-3E46-4541-A374-4EC13FC6C075}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{C6E18974-3E46-4541-A374-4EC13FC6C075}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Según lo estudiado en el artículo Design Principles and Top Non-Fullerene Acceptor Candidates for Organic Photovoltaics, vemos que se sigue la siguiente secuencia en la ejecución que lleva a las móleculas deseadas:</t>
-  </si>
-  <si>
-    <t>Es así que a través de unas móleculas definidad con anterioridad, las cuales se encuentran en el Data S1, en el siguiente enlace https://doi.org/10.1016/j.joule.2017.10.006. Se procede a realizar con los smiles descritos en la tabla S1, una muestra de conformers, los cuales se busca su minimal local energy a través de méthodos de mecánica molecular tal como el force field, que busca la reducción de la energía total descrita en la fórmula siguiente:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Texto</t>
   </si>
@@ -70,18 +58,6 @@
   </si>
   <si>
     <t>[E_{es} \]</t>
-  </si>
-  <si>
-    <t>Donde:
-\begin{fleqn}
-\begin{equation*}
-\begin{alignedat}{2}
-\\ &amp;k_b = bond-stretching \ force \ constant \\  
-&amp;r = actual\ bond\ length \\ 
-&amp;r_0 = defines\ equilibrium\ length\\
-\end{alignedat}
-\end{equation*}
-\end{fleqn}</t>
   </si>
   <si>
     <t>\begin{equation}
@@ -94,12 +70,6 @@
 \end{equation}</t>
   </si>
   <si>
-    <t>Como podemos ver en la fígura 2, y por la ecuación 2, lo ideal es disminuir la longitud actual de los enlaces a la longitud de equilibrio (la biografía y método para hallarla se encuentra en el siguiente \href{https://chem.libretexts.org/Bookshelves/Physical_and_Theoretical_Chemistry_Textbook_Maps/Supplemental_Modules_(Physical_and_Theoretical_Chemistry)/Chemical_Bonding/Fundamentals_of_Chemical_Bonding/Bond_Order_and_Lengths}{enlace}. Ahora para la Angle Bending Energy, $E_{bend}$ se encuentra su valor a través de la fórmula:</t>
-  </si>
-  <si>
-    <t>Donde tenemos que para la stretching energy $E_{str}$ se encuentra su valor a través de la fórmula (Cabe resaltar que la siguiente fórmula no se usa en los métodos cómo MMFF94, donde se términos cuadráticos y cúbicos):</t>
-  </si>
-  <si>
     <t>\begin{equation}
     E_{bend} = \frac{1}{2} \sum_{angles} k_\theta (\theta - \theta_0)^2
 \end{equation}</t>
@@ -108,14 +78,31 @@
     <t>preguntas</t>
   </si>
   <si>
-    <t>¿La razón por la cual se crean conformers en un inicio, es para dar diferentes configuraciones desde las cuales al aplicar el MMFF se logre una mayor probabilidad de encontrar el mínimo global de la energía?</t>
+    <t>Las células solares orgánicas nos muestran un camino interesante hacia el uso de energías renovables ecológicas y amigables. Eso nos ayudará a mitigar el efecto o huella de carbono. Se están cuestionando formas eficientes de convertir la energía solar en electricidad, como el uso de materiales, buscando las mejores propiedades que permitan una óptima conversión energética. Este trabajo explora el uso de técnicas de aprendizaje automático (ML) para ayudar a optimizar propiedades moleculares como el orbital molecular de alta ocupación (HOMO) y las energías de orbital molecular desocupado más bajo (LUMO), así como el cálculo y calibración de la eficiencia de conversión de potencia (PCE). ) con el ánimo de buscar grandes candidatas a moléculas orgánicas para su uso como sistemas donante-receptor en células solares. En particular, probamos una calibración del proceso gaussiano como un modelo ML en un conjunto de moléculas reportadas en la literatura [1] y discutimos algunos aspectos tanto de las propiedades químicas como de la ventaja de usar ML</t>
+  </si>
+  <si>
+    <r>
+      <t>Keywords:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Organic Solar Cell, Small Molecules, Machine Learning, Computational Chemistry, Quantum Systems.</t>
+    </r>
+  </si>
+  <si>
+    <t>ORCA es un programa flexible para química computacional que hace especial énfasis en propiedades espectroscópicas de moléculas de capa abierta. Trata una gran variedad de métodos de química cuántica desde métodos semiempíricos, la teoría del funcional de la densidad (Density Functional Theory, DFT), hasta métodos ab initio simples y de multireferencia, así como efectos relativísticos y medioambientales.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +116,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -172,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -192,6 +193,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +214,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -509,10 +513,10 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="91.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
@@ -523,91 +527,84 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
       <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrega imagen de demo en computacion y avances
</commit_message>
<xml_diff>
--- a/docs/textAvance.xlsx
+++ b/docs/textAvance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff2dc98e2a8f9132/University Proyect/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{174778ED-BF3D-42A4-A245-062591C956B6}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{7DC7D18E-251B-4AEF-96CE-E4F5582B8889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B9E5F2B-026B-4900-B30B-9A816E5CF198}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{C6E18974-3E46-4541-A374-4EC13FC6C075}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Texto</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>ORCA es un programa flexible para química computacional que hace especial énfasis en propiedades espectroscópicas de moléculas de capa abierta. Trata una gran variedad de métodos de química cuántica desde métodos semiempíricos, la teoría del funcional de la densidad (Density Functional Theory, DFT), hasta métodos ab initio simples y de multireferencia, así como efectos relativísticos y medioambientales.</t>
+  </si>
+  <si>
+    <t>Para la ejecución de la solución presentada en el artículo se utilizaron las bases def2-SVP y los métodos BP86 y B3LYP, al consultar la documentación se encuentran todos disponibles, sin embargo una de las bases no se encuentra tal como la muestra el artículo, por lo que mientras se soluciona, se opta por utilizar en ambas la def2-SVP, la otra base era double-z def2-SVP</t>
+  </si>
+  <si>
+    <t>Como se muestra en la anterior imágen el uso de orca para este sistema es simple en escritura, el paso posterior luego de comprobado que funciona la instalación, fue comunicar con el archivo en colab, sin embargo se encuentra en fase de despliegue del programa de orca para este proposito.</t>
   </si>
 </sst>
 </file>
@@ -512,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123720D3-AFD9-4B01-AE0E-0EAED385E34E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,15 +578,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
         <v>7</v>

</xml_diff>